<commit_message>
"optimized version of a solution to the problem 2  in Task B"
</commit_message>
<xml_diff>
--- a/mmc/data/dispatch_result_multi.xlsx
+++ b/mmc/data/dispatch_result_multi.xlsx
@@ -451,14 +451,14 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>moved_out</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>to</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>moved_out</t>
-        </is>
-      </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
           <t>moved_in</t>
@@ -471,7 +471,7 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>nij_score</t>
+          <t>nij</t>
         </is>
       </c>
     </row>
@@ -487,13 +487,13 @@
           <t>北门</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>教学2楼</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>二食堂</t>
+        </is>
       </c>
       <c r="F2" t="n">
         <v>20</v>
@@ -502,7 +502,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.617044273434094</v>
+        <v>0.4283840080205571</v>
       </c>
     </row>
     <row r="3">
@@ -517,22 +517,22 @@
           <t>菊苑1栋</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>教学2楼</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>二食堂</t>
+        </is>
       </c>
       <c r="F3" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G3" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5523796160379261</v>
+        <v>0.5017841360825993</v>
       </c>
     </row>
     <row r="4">
@@ -544,25 +544,25 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>教学2楼</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>工程中心</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
+          <t>二食堂</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>一食堂</t>
+        </is>
       </c>
       <c r="F4" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1768802480810299</v>
+        <v>0.3948432400342524</v>
       </c>
     </row>
     <row r="5">
@@ -574,25 +574,25 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>南门</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>教学4楼</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
+          <t>东门</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>三食堂</t>
+        </is>
       </c>
       <c r="F5" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="G5" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>0.2298262732773886</v>
+        <v>0.4205826887426308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>